<commit_message>
Work on insulation creation continues
</commit_message>
<xml_diff>
--- a/MyRevitAddins/MEPUtils/Insulation.xlsx
+++ b/MyRevitAddins/MEPUtils/Insulation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>BK</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>System</t>
+  </si>
+  <si>
+    <t>Isover Tapelock Rørskål</t>
   </si>
 </sst>
 </file>
@@ -427,10 +430,13 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -486,6 +492,9 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" s="1">
         <v>20</v>
       </c>
@@ -533,6 +542,9 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="1">
         <v>20</v>
       </c>
@@ -580,6 +592,9 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="1">
         <v>20</v>
       </c>
@@ -627,6 +642,9 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="1">
         <v>30</v>
       </c>
@@ -674,6 +692,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="1">
         <v>20</v>
       </c>
@@ -721,6 +742,9 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
       <c r="C7" s="1">
         <v>20</v>
       </c>
@@ -768,6 +792,9 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
       <c r="C8" s="1">
         <v>20</v>
       </c>
@@ -815,6 +842,9 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
       <c r="C9" s="1">
         <v>20</v>
       </c>
@@ -862,6 +892,9 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="1">
         <v>20</v>
       </c>
@@ -909,6 +942,9 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
       <c r="C11" s="1">
         <v>20</v>
       </c>
@@ -956,6 +992,9 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
       <c r="C12" s="1">
         <v>20</v>
       </c>
@@ -1003,6 +1042,9 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" s="1">
         <v>20</v>
       </c>
@@ -1050,6 +1092,9 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="1">
         <v>20</v>
       </c>
@@ -1096,6 +1141,9 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>

</xml_diff>